<commit_message>
msz - ready for next video part 2 ;-)
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgPasswordReset.xlsx
+++ b/Data/Dialogs/dlgPasswordReset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2453CA45-EFE1-488C-A948-1241BAA9878D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68493074-AD8E-4B2A-AB0D-B94AED5D5DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="37188" windowHeight="15300" xr2:uid="{C8A25197-C6D3-4075-A8EF-C8E1E24C2FC4}"/>
+    <workbookView xWindow="336" yWindow="564" windowWidth="39240" windowHeight="15768" xr2:uid="{C8A25197-C6D3-4075-A8EF-C8E1E24C2FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>altFehler</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t xml:space="preserve">Record / Control </t>
+  </si>
+  <si>
+    <t>//android.view.View[@content-desc="TT-Planer"]</t>
+  </si>
+  <si>
+    <t>//android.widget.EditText[@resource-id="email"]</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@text="Passwort zurücksetzen Link schicken"]</t>
+  </si>
+  <si>
+    <t>//android.widget.TextView[@text="Zurück zum Login"]</t>
   </si>
 </sst>
 </file>
@@ -141,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +172,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -173,11 +191,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -205,8 +224,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>604559</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>353099</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>45120</xdr:rowOff>
     </xdr:to>
@@ -544,20 +563,20 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="H22" sqref="H21:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
     <col min="5" max="5" width="46.21875" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" customWidth="1"/>
+    <col min="7" max="7" width="42" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -599,13 +618,21 @@
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="J2" t="s">
         <v>4</v>
       </c>

</xml_diff>